<commit_message>
Inicio de configuracion para mas variables
</commit_message>
<xml_diff>
--- a/EJEMPLO.xlsx
+++ b/EJEMPLO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADM1\Desktop\Facturador-test-casa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADM1\Desktop\Programas\Facturador Completo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>CUIT</t>
   </si>
@@ -58,6 +58,21 @@
   </si>
   <si>
     <t>Varios</t>
+  </si>
+  <si>
+    <t>CUIT Receptor</t>
+  </si>
+  <si>
+    <t>Alicuota</t>
+  </si>
+  <si>
+    <t>Condicion Receptor</t>
+  </si>
+  <si>
+    <t>Consumidor Final</t>
+  </si>
+  <si>
+    <t>21%</t>
   </si>
 </sst>
 </file>
@@ -118,7 +133,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -128,6 +143,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,19 +424,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -428,39 +447,46 @@
         <v>6</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>45377</v>
+        <v>45401</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2">
+        <v>20391117471</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="D2">
+      <c r="G2">
         <v>114200</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>45377</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3">
-        <v>116900</v>
-      </c>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -472,7 +498,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>